<commit_message>
done first two modes
</commit_message>
<xml_diff>
--- a/inst.xlsx
+++ b/inst.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="99">
   <si>
     <t xml:space="preserve">immediate</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve"># # # # # # # #</t>
   </si>
   <si>
+    <t xml:space="preserve">ldr r1, #h01</t>
+  </si>
+  <si>
     <t xml:space="preserve">add</t>
   </si>
   <si>
@@ -121,7 +124,7 @@
     <t xml:space="preserve">10010 r r r</t>
   </si>
   <si>
-    <t xml:space="preserve">register register address</t>
+    <t xml:space="preserve">register register</t>
   </si>
   <si>
     <t xml:space="preserve">FF</t>
@@ -247,24 +250,12 @@
     <t xml:space="preserve">E4</t>
   </si>
   <si>
-    <t xml:space="preserve">jb</t>
+    <t xml:space="preserve">call</t>
   </si>
   <si>
     <t xml:space="preserve">E3</t>
   </si>
   <si>
-    <t xml:space="preserve">jnb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">call</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1</t>
-  </si>
-  <si>
     <t xml:space="preserve">only register</t>
   </si>
   <si>
@@ -322,7 +313,7 @@
     <t xml:space="preserve">11011 r r r</t>
   </si>
   <si>
-    <t xml:space="preserve">hlt</t>
+    <t xml:space="preserve">ret</t>
   </si>
   <si>
     <t xml:space="preserve">E0</t>
@@ -335,12 +326,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -359,12 +349,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -415,7 +399,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,10 +409,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,14 +432,14 @@
   </sheetPr>
   <dimension ref="A2:D101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
   </cols>
   <sheetData>
@@ -478,13 +458,16 @@
       <c r="C3" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>3</v>
@@ -492,10 +475,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>3</v>
@@ -503,10 +486,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>3</v>
@@ -514,10 +497,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>3</v>
@@ -525,10 +508,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>3</v>
@@ -536,10 +519,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>3</v>
@@ -547,10 +530,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>3</v>
@@ -558,10 +541,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>3</v>
@@ -569,7 +552,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,144 +560,144 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,114 +705,114 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,357 +820,329 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="3"/>
+      <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -1196,10 +1151,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C73" s="2"/>
     </row>

</xml_diff>

<commit_message>
first 4 modes done
</commit_message>
<xml_diff>
--- a/inst.xlsx
+++ b/inst.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="98">
   <si>
     <t xml:space="preserve">immediate</t>
   </si>
@@ -157,103 +157,100 @@
     <t xml:space="preserve">F7</t>
   </si>
   <si>
+    <t xml:space="preserve">register register indirect 16bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000 r r r r r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE</t>
+  </si>
+  <si>
     <t xml:space="preserve">str </t>
   </si>
   <si>
-    <t xml:space="preserve">F6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">register register indirect 16bits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">000 r r r r r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE</t>
-  </si>
-  <si>
     <t xml:space="preserve">ED</t>
   </si>
   <si>
+    <t xml:space="preserve">only address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmp</t>
+  </si>
+  <si>
     <t xml:space="preserve">EC</t>
   </si>
   <si>
-    <t xml:space="preserve">only address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jmp</t>
+    <t xml:space="preserve">jz</t>
   </si>
   <si>
     <t xml:space="preserve">EB</t>
   </si>
   <si>
-    <t xml:space="preserve">jz</t>
+    <t xml:space="preserve">je</t>
   </si>
   <si>
     <t xml:space="preserve">EA</t>
   </si>
   <si>
-    <t xml:space="preserve">je</t>
+    <t xml:space="preserve">jne</t>
   </si>
   <si>
     <t xml:space="preserve">E9</t>
   </si>
   <si>
-    <t xml:space="preserve">jne</t>
+    <t xml:space="preserve">jgt</t>
   </si>
   <si>
     <t xml:space="preserve">E8</t>
   </si>
   <si>
-    <t xml:space="preserve">jgt</t>
+    <t xml:space="preserve">jlt</t>
   </si>
   <si>
     <t xml:space="preserve">E7</t>
   </si>
   <si>
-    <t xml:space="preserve">jlt</t>
+    <t xml:space="preserve">jc</t>
   </si>
   <si>
     <t xml:space="preserve">E6</t>
   </si>
   <si>
-    <t xml:space="preserve">jc</t>
+    <t xml:space="preserve">jnc</t>
   </si>
   <si>
     <t xml:space="preserve">E5</t>
   </si>
   <si>
-    <t xml:space="preserve">jnc</t>
+    <t xml:space="preserve">call</t>
   </si>
   <si>
     <t xml:space="preserve">E4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">call</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E3</t>
   </si>
   <si>
     <t xml:space="preserve">only register</t>
@@ -331,6 +328,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -352,6 +350,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -432,11 +431,11 @@
   </sheetPr>
   <dimension ref="A2:D101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
@@ -799,20 +798,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,10 +808,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,10 +819,10 @@
         <v>5</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,10 +830,10 @@
         <v>7</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,10 +841,10 @@
         <v>9</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,10 +852,10 @@
         <v>11</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,10 +863,10 @@
         <v>13</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,10 +874,10 @@
         <v>15</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,10 +885,10 @@
         <v>17</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,34 +896,34 @@
         <v>19</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>23</v>
@@ -946,10 +934,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>23</v>
@@ -960,10 +948,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>23</v>
@@ -974,10 +962,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>23</v>
@@ -988,10 +976,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>23</v>
@@ -1002,10 +990,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>23</v>
@@ -1016,10 +1004,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>23</v>
@@ -1030,10 +1018,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>23</v>
@@ -1044,10 +1032,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>23</v>
@@ -1062,87 +1050,87 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>84</v>
       </c>
       <c r="C65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="C66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="C67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="C68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="C69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="C70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -1151,10 +1139,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="C73" s="2"/>
     </row>

</xml_diff>